<commit_message>
data checked and inserted.
</commit_message>
<xml_diff>
--- a/static/MedicineUploads/MedicneStoreExpirySearchList.xlsx
+++ b/static/MedicineUploads/MedicneStoreExpirySearchList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="147">
   <si>
     <t>Drug Name</t>
   </si>
@@ -37,151 +37,424 @@
     <t>RackNumber</t>
   </si>
   <si>
-    <t>ALLOPURINOL-100 MG</t>
+    <t>PARACETAMOL PAEDIATRIC SYR 60 ML</t>
+  </si>
+  <si>
+    <t>Syrup</t>
+  </si>
+  <si>
+    <t>SO180055</t>
+  </si>
+  <si>
+    <t>01-10-2018</t>
+  </si>
+  <si>
+    <t>30-09-2020</t>
+  </si>
+  <si>
+    <t>649</t>
+  </si>
+  <si>
+    <t>S1 L2</t>
+  </si>
+  <si>
+    <t>ANTACID TABLETS</t>
   </si>
   <si>
     <t>Tablet</t>
   </si>
   <si>
-    <t>AKT2073</t>
+    <t>ZD1811029</t>
+  </si>
+  <si>
+    <t>30-09-2018</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>AZYTHROMYCIN 500 MG</t>
+  </si>
+  <si>
+    <t>8443017</t>
+  </si>
+  <si>
+    <t>Heparin  25000 unit  INJ 5 ML</t>
+  </si>
+  <si>
+    <t>Injection</t>
+  </si>
+  <si>
+    <t>IHEPB1828</t>
   </si>
   <si>
     <t>31-10-2018</t>
   </si>
   <si>
-    <t>31-10-2019</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>HALOPERIDOL  5 MG (serenes)</t>
-  </si>
-  <si>
-    <t>LOT27S17015</t>
-  </si>
-  <si>
-    <t>30-10-2019</t>
-  </si>
-  <si>
-    <t>MEBENDAZOLE  100 MG</t>
-  </si>
-  <si>
-    <t>001A8ABC</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>SR1</t>
+  </si>
+  <si>
+    <t>TRAMSULOSIN HYDROCHLORIDE 0.4 MG  AND FINASTERIDE 5 MG</t>
+  </si>
+  <si>
+    <t>Capsule</t>
+  </si>
+  <si>
+    <t>FT181105</t>
+  </si>
+  <si>
+    <t>30-09-2019</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>BECLAMETHASONE NEOMYCIN SULPHATE OINT LC 15 G</t>
+  </si>
+  <si>
+    <t>Ointment</t>
+  </si>
+  <si>
+    <t>B390</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
+    <t>S4 L1</t>
+  </si>
+  <si>
+    <t>IBUPROFEN PARACETAMOL 400 MG</t>
+  </si>
+  <si>
+    <t>C171217</t>
+  </si>
+  <si>
+    <t>HALOTHANE B.P. 250 ML</t>
+  </si>
+  <si>
+    <t>NP573002</t>
+  </si>
+  <si>
+    <t>31-10-2016</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>VITAMIN B COMPLEX LC</t>
+  </si>
+  <si>
+    <t>PR4391R</t>
+  </si>
+  <si>
+    <t>01-04-2019</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BISACODYL SUPPOSITORIES IP 10 MG </t>
+  </si>
+  <si>
+    <t>T701079</t>
+  </si>
+  <si>
+    <t>31-12-2016</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>INDOMETHACINE 25 MG</t>
+  </si>
+  <si>
+    <t>6107</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>S3 L3</t>
+  </si>
+  <si>
+    <t>METFORMIN HYDROCHLORIDE-500 MG</t>
+  </si>
+  <si>
+    <t>IZD16033</t>
   </si>
   <si>
     <t>30-10-2018</t>
   </si>
   <si>
-    <t xml:space="preserve">PENICILLIN G POTASSIUM   400 MG </t>
-  </si>
-  <si>
-    <t>VVD0226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIFAMPICIN AND ISONICID CAPSULES USP 450 plus 300MG  </t>
-  </si>
-  <si>
-    <t>Capsule</t>
-  </si>
-  <si>
-    <t>A706979</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>Setraline HydroChrloride 50mg</t>
-  </si>
-  <si>
-    <t>HT3073</t>
-  </si>
-  <si>
-    <t>METHYLERGOMETRINE INJ IP 1ML</t>
-  </si>
-  <si>
-    <t>Injection</t>
-  </si>
-  <si>
-    <t>ILMI-002</t>
-  </si>
-  <si>
-    <t>30-04-2018</t>
-  </si>
-  <si>
-    <t>30-09-2019</t>
+    <t>2200</t>
+  </si>
+  <si>
+    <t>TR2 L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOSARTAN 50 MG                                  </t>
+  </si>
+  <si>
+    <t>ZD181045</t>
+  </si>
+  <si>
+    <t>TRANEXAMIC ACID INJECTION 5 ML</t>
+  </si>
+  <si>
+    <t>K80223</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>IR9 L</t>
+  </si>
+  <si>
+    <t>INSULINE INJ 40IU/ML</t>
+  </si>
+  <si>
+    <t>QT101443</t>
+  </si>
+  <si>
+    <t>31-08-2020</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BISACODYL SUPPOSITORIES IP 5 MG </t>
+  </si>
+  <si>
+    <t>1700939</t>
+  </si>
+  <si>
+    <t>30-09-2017</t>
   </si>
   <si>
     <t>45</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>SOYAL MILK</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>038D001</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>METFORMIN HYDROCHLORIDE-500 MG</t>
-  </si>
-  <si>
-    <t>IZD16033</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
-    <t>TR2 L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OFLOXACIN 200 MG                 </t>
-  </si>
-  <si>
-    <t>17NT1032</t>
-  </si>
-  <si>
-    <t>30-09-2018</t>
-  </si>
-  <si>
-    <t>QUETIAPINE          50 MG</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMOXICILLIN TRIHYDRATE T-125 </t>
-  </si>
-  <si>
-    <t>ASK7002R</t>
-  </si>
-  <si>
-    <t>31-08-2018</t>
-  </si>
-  <si>
-    <t>31-08-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METOCLOPROMAMIDE HYDROCHLORIC 10 Mg         </t>
-  </si>
-  <si>
-    <t>T1709192</t>
+    <t>Progesteron 100 MG</t>
+  </si>
+  <si>
+    <t>DM660</t>
+  </si>
+  <si>
+    <t>30-08-2020</t>
+  </si>
+  <si>
+    <t>AMIODARONE INTRAVENOUS INJ 3 ML</t>
+  </si>
+  <si>
+    <t>8A096</t>
+  </si>
+  <si>
+    <t>01-09-2018</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>IR7 L</t>
+  </si>
+  <si>
+    <t>INSULIN REGULAR INJ 10 ML</t>
+  </si>
+  <si>
+    <t>QT10143</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>POTASSIUM CHLORIDE INJ 10 ML</t>
+  </si>
+  <si>
+    <t>PC-212</t>
+  </si>
+  <si>
+    <t>GLIMEPERIDE TABLET 2 MG</t>
+  </si>
+  <si>
+    <t>PPKAJ03</t>
   </si>
   <si>
     <t>30-08-2019</t>
+  </si>
+  <si>
+    <t>CLOPIDOGRAL TABLETS 75 MG</t>
+  </si>
+  <si>
+    <t>MOT18557</t>
+  </si>
+  <si>
+    <t>RAMIPRIL TABLETS 5 MG</t>
+  </si>
+  <si>
+    <t>BA83472</t>
+  </si>
+  <si>
+    <t>CLOMIFEN 25 MG</t>
+  </si>
+  <si>
+    <t>SA74279</t>
+  </si>
+  <si>
+    <t>30-08-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VITAMIN A AND D </t>
+  </si>
+  <si>
+    <t>VTF1808073</t>
+  </si>
+  <si>
+    <t>CR1</t>
+  </si>
+  <si>
+    <t>HYDROCHLOROTHIAZIDE TAB 25 MG</t>
+  </si>
+  <si>
+    <t>OVTE1883</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>TPPKAJ03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENAPRIL MALEAT 5 MG                  </t>
+  </si>
+  <si>
+    <t>V801009</t>
+  </si>
+  <si>
+    <t>TRANEXAMIC ACID  500 MG</t>
+  </si>
+  <si>
+    <t>AKT3545</t>
+  </si>
+  <si>
+    <t>VHF18073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERBINAFINE HYDROCHLORIDE CREAM 15 G </t>
+  </si>
+  <si>
+    <t>0746</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>R6 L2</t>
+  </si>
+  <si>
+    <t>CLOTRIMAZOLE VAGINAL TABLETS 100MG</t>
+  </si>
+  <si>
+    <t>ZD18776</t>
+  </si>
+  <si>
+    <t>31-07-2019</t>
+  </si>
+  <si>
+    <t>31-07-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACICLOVIR TABLETS  400mg                </t>
+  </si>
+  <si>
+    <t>VPT-18411D</t>
+  </si>
+  <si>
+    <t>31-07-2018</t>
+  </si>
+  <si>
+    <t>30-07-2020</t>
+  </si>
+  <si>
+    <t>TR1 L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICLOXACILLIN SODIUM  250 MG  </t>
+  </si>
+  <si>
+    <t>KD1902001</t>
+  </si>
+  <si>
+    <t>30-07-2019</t>
+  </si>
+  <si>
+    <t>DICLOXACILLIAN SODIUM CAPS 500MG</t>
+  </si>
+  <si>
+    <t>28-02-2019</t>
+  </si>
+  <si>
+    <t>CR3 L</t>
+  </si>
+  <si>
+    <t>DIGOXIN  0.25 MG</t>
+  </si>
+  <si>
+    <t>T-11669</t>
+  </si>
+  <si>
+    <t>MUCAINE GEL SYR 200 ML</t>
+  </si>
+  <si>
+    <t>ZA18495</t>
+  </si>
+  <si>
+    <t>01-08-2018</t>
+  </si>
+  <si>
+    <t>S2 L1</t>
+  </si>
+  <si>
+    <t>AMOXICILLIN CAPSULES 500 MG</t>
+  </si>
+  <si>
+    <t>0088PB011</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>C3 L1</t>
+  </si>
+  <si>
+    <t>DOMPERIDOM  10 MG</t>
+  </si>
+  <si>
+    <t>ZT1808</t>
+  </si>
+  <si>
+    <t>RANITIDINE HYDROCHLORIDE INJ 2ML</t>
+  </si>
+  <si>
+    <t>ULN1869</t>
+  </si>
+  <si>
+    <t>30-06-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR10 </t>
   </si>
 </sst>
 </file>
@@ -522,7 +795,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -579,298 +852,965 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E36" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" t="s">
+        <v>123</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>126</v>
+      </c>
+      <c r="D38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" t="s">
+        <v>123</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" t="s">
+        <v>127</v>
+      </c>
+      <c r="E40" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>13</v>
+      <c r="C41" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" t="s">
+        <v>123</v>
+      </c>
+      <c r="F41" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" t="s">
+        <v>123</v>
+      </c>
+      <c r="F42" t="s">
+        <v>139</v>
+      </c>
+      <c r="G42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" t="s">
+        <v>135</v>
+      </c>
+      <c r="E43" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" t="s">
+        <v>145</v>
+      </c>
+      <c r="E44" t="s">
+        <v>123</v>
+      </c>
+      <c r="F44" t="s">
+        <v>72</v>
+      </c>
+      <c r="G44" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>